<commit_message>
created files to read data fromexcel
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\SauceDemoFirstGroup2024\src\test\java\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nkosi/Documents/ClassProjects/3rdGroup2024SeleniumJava/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7569681-10A0-48FC-A660-DDB0D0F9F4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1655E9A-801F-D142-A0D5-6086B7707104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7960" yWindow="6220" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information Tab" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>problem_user</t>
+  </si>
+  <si>
+    <t>Cele</t>
+  </si>
+  <si>
+    <t>Nkosi</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -406,17 +412,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A607" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E612" sqref="E612"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -424,7 +430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -432,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -440,7 +446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -448,22 +454,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created code to read username and password from excel file
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nkosi/Documents/ClassProjects/3rdGroup2024SeleniumJava/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1655E9A-801F-D142-A0D5-6086B7707104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79730C67-4335-554D-80A1-C801B8597617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="6220" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10340" yWindow="5760" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information Tab" sheetId="2" r:id="rId1"/>
@@ -34,22 +34,22 @@
     <t>Password</t>
   </si>
   <si>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
+  </si>
+  <si>
+    <t>problem_user</t>
+  </si>
+  <si>
+    <t>Cele</t>
+  </si>
+  <si>
+    <t>Nkosi</t>
+  </si>
+  <si>
     <t>standard_user</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
-  </si>
-  <si>
-    <t>problem_user</t>
-  </si>
-  <si>
-    <t>Cele</t>
-  </si>
-  <si>
-    <t>Nkosi</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A607" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E612" sqref="E612"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -432,44 +432,44 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Tests for Assessment Question 1 to Question 18.
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nkosi/Documents/ClassProjects/3rdGroup2024SeleniumJava/src/test/java/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dd9e82c5c5fc1f06/Documents/3rdGroup2024SeleniumJava/src/test/java/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79730C67-4335-554D-80A1-C801B8597617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{79730C67-4335-554D-80A1-C801B8597617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C671AADB-9A45-4C04-AD3F-C862C8ED8FB0}"/>
   <bookViews>
-    <workbookView xWindow="10340" yWindow="5760" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information Tab" sheetId="2" r:id="rId1"/>
@@ -402,7 +402,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -416,13 +416,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -430,7 +430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -438,7 +438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -454,19 +454,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>6</v>

</xml_diff>